<commit_message>
Arreglo del indice de proyectos empréstito
</commit_message>
<xml_diff>
--- a/transformation_app/app_inputs/unidades_proyecto_input/obras_lineales.xlsx
+++ b/transformation_app/app_inputs/unidades_proyecto_input/obras_lineales.xlsx
@@ -5,17 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\programing_workspace\api-dashboard-db\transformation_app\app_inputs\unidades_proyecto_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\programing_workspace\proyectos_cali_alcaldia_etl\transformation_app\app_inputs\unidades_proyecto_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09269B4-BAC2-4758-BD87-98496046E65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA203D30-796C-42CE-AC79-897AE40CC116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="obra_lineal" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1582,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>